<commit_message>
Updated supplier prequalification report
</commit_message>
<xml_diff>
--- a/src/private/templates/suppliers_prequalification.xlsx
+++ b/src/private/templates/suppliers_prequalification.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Supplier</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Business integrity</t>
   </si>
@@ -39,13 +36,31 @@
   </si>
   <si>
     <t>Finance</t>
+  </si>
+  <si>
+    <t>Supplier Name</t>
+  </si>
+  <si>
+    <t>Vendor Number</t>
+  </si>
+  <si>
+    <t>Prequalification status</t>
+  </si>
+  <si>
+    <t>Expiry date</t>
+  </si>
+  <si>
+    <t>Tier type</t>
+  </si>
+  <si>
+    <t>Suppliers pre-qualification report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,18 +68,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="161"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="161"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <charset val="161"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF969696"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -74,8 +141,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -85,6 +177,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -353,36 +448,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
+      <selection activeCell="J1" sqref="A1:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" s="8" customFormat="1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>